<commit_message>
print up to four codes per pdf.
</commit_message>
<xml_diff>
--- a/lankar.xlsx
+++ b/lankar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christoffer.rydestah\Documents\Repos\QR-code-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102AADA5-7F1C-4BB2-B235-090B93BE5DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7990AB2E-C7C7-49C9-86FD-B3898B286CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5640" yWindow="1770" windowWidth="21600" windowHeight="11295" xr2:uid="{5B7EDCFC-7894-45D4-A6CC-EB5598027E1C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>https://www.svt.se/</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>https://gaffa.se/</t>
+  </si>
+  <si>
+    <t>https://www.nordea.se/</t>
+  </si>
+  <si>
+    <t>https://www.aftonbladet.se/</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A032883D-987B-4019-B61D-EAD06BF8FC10}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,6 +461,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>